<commit_message>
Finished intial part with data
</commit_message>
<xml_diff>
--- a/data/DF.xlsx
+++ b/data/DF.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP11"/>
+  <dimension ref="A1:AP12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -993,8 +993,12 @@
       <c r="I5" t="n">
         <v>42.51272258583246</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
       <c r="L5" t="n">
         <v>19.38</v>
       </c>
@@ -1019,14 +1023,18 @@
       <c r="S5" t="n">
         <v>26.67587011635359</v>
       </c>
-      <c r="T5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
       <c r="U5" t="n">
         <v>72.52</v>
       </c>
       <c r="V5" t="n">
         <v>78.01451919758264</v>
       </c>
-      <c r="W5" t="inlineStr"/>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
       <c r="X5" t="n">
         <v>91.47929619999999</v>
       </c>
@@ -1066,11 +1074,15 @@
       <c r="AJ5" t="n">
         <v>0.2</v>
       </c>
-      <c r="AK5" t="inlineStr"/>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
       <c r="AL5" t="n">
         <v>20.18300000000001</v>
       </c>
-      <c r="AM5" t="inlineStr"/>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
       <c r="AN5" t="n">
         <v>1759540</v>
       </c>
@@ -1223,7 +1235,9 @@
       <c r="C7" t="n">
         <v>42.9123191833496</v>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
       <c r="E7" t="n">
         <v>82.61883544921881</v>
       </c>
@@ -1686,7 +1700,9 @@
       <c r="AB10" t="n">
         <v>3.53520683416771</v>
       </c>
-      <c r="AC10" t="inlineStr"/>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
       <c r="AD10" t="n">
         <v>2.39521985845548</v>
       </c>
@@ -1717,7 +1733,9 @@
       <c r="AM10" t="n">
         <v>46.79085376604269</v>
       </c>
-      <c r="AN10" t="inlineStr"/>
+      <c r="AN10" t="n">
+        <v>0</v>
+      </c>
       <c r="AO10" t="n">
         <v>34.37</v>
       </c>
@@ -1855,7 +1873,137 @@
         <v>1.571234060855332</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>88.84863805865645</v>
+      </c>
+      <c r="D12" t="n">
+        <v>78.64735578125527</v>
+      </c>
+      <c r="E12" t="n">
+        <v>97.35769156507307</v>
+      </c>
+      <c r="F12" t="n">
+        <v>42.45569899944301</v>
+      </c>
+      <c r="G12" t="n">
+        <v>54.21683086088953</v>
+      </c>
+      <c r="H12" t="n">
+        <v>13.21604411832126</v>
+      </c>
+      <c r="I12" t="n">
+        <v>39.6440809675836</v>
+      </c>
+      <c r="J12" t="n">
+        <v>3.418853897824389</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.8038986377878641</v>
+      </c>
+      <c r="L12" t="n">
+        <v>18.65693389189641</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7.54240423884828</v>
+      </c>
+      <c r="N12" t="n">
+        <v>28.40931040761491</v>
+      </c>
+      <c r="O12" t="n">
+        <v>23.07488912516291</v>
+      </c>
+      <c r="P12" t="n">
+        <v>48.51578710374548</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2.431584662931561</v>
+      </c>
+      <c r="R12" t="n">
+        <v>80891341462319.14</v>
+      </c>
+      <c r="S12" t="n">
+        <v>3.165402310413128</v>
+      </c>
+      <c r="T12" t="n">
+        <v>25.50045483934074</v>
+      </c>
+      <c r="U12" t="n">
+        <v>72.38300866126713</v>
+      </c>
+      <c r="V12" t="n">
+        <v>44.47336011088299</v>
+      </c>
+      <c r="W12" t="n">
+        <v>2.161438045828547</v>
+      </c>
+      <c r="X12" t="n">
+        <v>102.7759657782136</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>25.93487403210847</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>65.41928443397815</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>8.645841533913378</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>58.97696677271883</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>1.143092581314392</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>16.09383079924788</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.4750067445347668</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>3722940052</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>3785204133</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>7510990456</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>45.17775825906573</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>65.03571648102344</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>132036620.8118786</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>54.8222417409343</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>1.98513545849886</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>